<commit_message>
changed PS3 alternate exploit
</commit_message>
<xml_diff>
--- a/list/summary.xlsx
+++ b/list/summary.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Files\Documents\GitHub\pauzen\list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60039EA7-3958-4891-A913-5BD1CF34DE14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4CEDC9-94FA-4BD7-8E09-5A1199A47688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="B3VKrvmqWGlQhOIYSpWaBRkfWom5KSRILRQXebpfLBWAYiZxgzxRSD0mGJB7axxwdqVXRNL1HWApoQ/7vxhrwQ==" workbookSaltValue="CuZ8B/bfQPuOM3LIrCafkA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="877" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="3396" windowWidth="17280" windowHeight="9072" tabRatio="877" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="38" state="hidden" r:id="rId1"/>
@@ -2038,42 +2038,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2092,6 +2061,37 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="34">
@@ -12697,7 +12697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56498E0-33C8-45FE-96EE-AC46EA23481D}">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
@@ -15927,19 +15927,19 @@
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="2:27" ht="13.8">
-      <c r="B2" s="179"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
-      <c r="L2" s="180"/>
-      <c r="M2" s="180"/>
-      <c r="N2" s="180"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
+      <c r="M2" s="193"/>
+      <c r="N2" s="193"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -15949,21 +15949,21 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="18.600000000000001">
-      <c r="B3" s="181" t="s">
+      <c r="B3" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="182"/>
-      <c r="N3" s="182"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="195"/>
+      <c r="N3" s="195"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -15973,21 +15973,21 @@
       </c>
     </row>
     <row r="4" spans="2:27" ht="13.8">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
-      <c r="K4" s="184"/>
-      <c r="L4" s="184"/>
-      <c r="M4" s="184"/>
-      <c r="N4" s="184"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -15997,21 +15997,21 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8">
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
+      <c r="F5" s="178"/>
+      <c r="G5" s="178"/>
+      <c r="H5" s="178"/>
+      <c r="I5" s="178"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="178"/>
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -16043,21 +16043,21 @@
       </c>
     </row>
     <row r="7" spans="2:27">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="178"/>
-      <c r="L7" s="178"/>
-      <c r="M7" s="178"/>
-      <c r="N7" s="178"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
+      <c r="L7" s="191"/>
+      <c r="M7" s="191"/>
+      <c r="N7" s="191"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -16083,11 +16083,11 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="2:27" ht="16.8">
-      <c r="B9" s="183" t="s">
+      <c r="B9" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="184"/>
-      <c r="D9" s="184"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
       <c r="E9" s="187" t="s">
         <v>14</v>
       </c>
@@ -16129,11 +16129,11 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="2:27" ht="16.8">
-      <c r="B11" s="183" t="s">
+      <c r="B11" s="177" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="184"/>
-      <c r="D11" s="184"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="187"/>
       <c r="F11" s="187"/>
       <c r="G11" s="187"/>
@@ -16150,42 +16150,42 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="2:27" ht="13.8">
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="184"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="184"/>
-      <c r="M12" s="184"/>
-      <c r="N12" s="184"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="178"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="178"/>
+      <c r="L12" s="178"/>
+      <c r="M12" s="178"/>
+      <c r="N12" s="178"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="2:27" ht="14.4" thickBot="1">
-      <c r="B13" s="190" t="s">
+      <c r="B13" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="191"/>
-      <c r="D13" s="191"/>
-      <c r="E13" s="191"/>
-      <c r="F13" s="191"/>
-      <c r="G13" s="191"/>
-      <c r="H13" s="191"/>
-      <c r="I13" s="191"/>
-      <c r="J13" s="191"/>
-      <c r="K13" s="191"/>
-      <c r="L13" s="191"/>
-      <c r="M13" s="191"/>
-      <c r="N13" s="191"/>
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="180"/>
+      <c r="M13" s="180"/>
+      <c r="N13" s="180"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -16195,10 +16195,10 @@
       <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="192" t="s">
+      <c r="C14" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="193"/>
+      <c r="D14" s="182"/>
       <c r="E14" s="86" t="s">
         <v>108</v>
       </c>
@@ -16236,8 +16236,8 @@
     </row>
     <row r="15" spans="2:27" hidden="1" thickBot="1">
       <c r="B15" s="11"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="195"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="184"/>
       <c r="E15" s="46"/>
       <c r="F15" s="46"/>
       <c r="G15" s="46"/>
@@ -19601,11 +19601,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:N12"/>
-    <mergeCell ref="B13:N13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B6:N6"/>
     <mergeCell ref="B8:N8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
@@ -19613,12 +19614,11 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="H11:N11"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:N12"/>
+    <mergeCell ref="B13:N13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <conditionalFormatting sqref="N16:N81">
     <cfRule type="cellIs" dxfId="31" priority="2" operator="greaterThan">
@@ -19688,19 +19688,19 @@
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="2:27" ht="13.8">
-      <c r="B2" s="179"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
-      <c r="L2" s="180"/>
-      <c r="M2" s="180"/>
-      <c r="N2" s="180"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
+      <c r="M2" s="193"/>
+      <c r="N2" s="193"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -19710,21 +19710,21 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="18.600000000000001">
-      <c r="B3" s="181" t="s">
+      <c r="B3" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="182"/>
-      <c r="N3" s="182"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="195"/>
+      <c r="N3" s="195"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -19734,21 +19734,21 @@
       </c>
     </row>
     <row r="4" spans="2:27" ht="13.8">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
-      <c r="K4" s="184"/>
-      <c r="L4" s="184"/>
-      <c r="M4" s="184"/>
-      <c r="N4" s="184"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -19758,21 +19758,21 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8">
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
+      <c r="F5" s="178"/>
+      <c r="G5" s="178"/>
+      <c r="H5" s="178"/>
+      <c r="I5" s="178"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="178"/>
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -19804,21 +19804,21 @@
       </c>
     </row>
     <row r="7" spans="2:27">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="178"/>
-      <c r="L7" s="178"/>
-      <c r="M7" s="178"/>
-      <c r="N7" s="178"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
+      <c r="L7" s="191"/>
+      <c r="M7" s="191"/>
+      <c r="N7" s="191"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -19844,11 +19844,11 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="2:27" ht="16.8">
-      <c r="B9" s="183" t="s">
+      <c r="B9" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="184"/>
-      <c r="D9" s="184"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
       <c r="E9" s="187" t="s">
         <v>14</v>
       </c>
@@ -19890,11 +19890,11 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="2:27" ht="16.8">
-      <c r="B11" s="183" t="s">
+      <c r="B11" s="177" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="184"/>
-      <c r="D11" s="184"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="187"/>
       <c r="F11" s="187"/>
       <c r="G11" s="187"/>
@@ -19911,42 +19911,42 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="2:27" ht="13.8">
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="184"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="184"/>
-      <c r="M12" s="184"/>
-      <c r="N12" s="184"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="178"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="178"/>
+      <c r="L12" s="178"/>
+      <c r="M12" s="178"/>
+      <c r="N12" s="178"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="2:27" ht="14.4" thickBot="1">
-      <c r="B13" s="190" t="s">
+      <c r="B13" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="191"/>
-      <c r="D13" s="191"/>
-      <c r="E13" s="191"/>
-      <c r="F13" s="191"/>
-      <c r="G13" s="191"/>
-      <c r="H13" s="191"/>
-      <c r="I13" s="191"/>
-      <c r="J13" s="191"/>
-      <c r="K13" s="191"/>
-      <c r="L13" s="191"/>
-      <c r="M13" s="191"/>
-      <c r="N13" s="191"/>
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="180"/>
+      <c r="M13" s="180"/>
+      <c r="N13" s="180"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -19956,10 +19956,10 @@
       <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="192" t="s">
+      <c r="C14" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="193"/>
+      <c r="D14" s="182"/>
       <c r="E14" s="86" t="s">
         <v>108</v>
       </c>
@@ -19997,8 +19997,8 @@
     </row>
     <row r="15" spans="2:27" hidden="1" thickBot="1">
       <c r="B15" s="11"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="195"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="184"/>
       <c r="E15" s="46"/>
       <c r="F15" s="46"/>
       <c r="G15" s="46"/>
@@ -23362,11 +23362,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:N12"/>
-    <mergeCell ref="B13:N13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B6:N6"/>
     <mergeCell ref="B8:N8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
@@ -23374,12 +23375,11 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="H11:N11"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:N12"/>
+    <mergeCell ref="B13:N13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <conditionalFormatting sqref="N16:N81">
     <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThan">
@@ -23449,19 +23449,19 @@
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="2:27" ht="13.8">
-      <c r="B2" s="179"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
-      <c r="L2" s="180"/>
-      <c r="M2" s="180"/>
-      <c r="N2" s="180"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
+      <c r="M2" s="193"/>
+      <c r="N2" s="193"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -23471,21 +23471,21 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="18.600000000000001">
-      <c r="B3" s="181" t="s">
+      <c r="B3" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="182"/>
-      <c r="N3" s="182"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="195"/>
+      <c r="N3" s="195"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -23495,21 +23495,21 @@
       </c>
     </row>
     <row r="4" spans="2:27" ht="13.8">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
-      <c r="K4" s="184"/>
-      <c r="L4" s="184"/>
-      <c r="M4" s="184"/>
-      <c r="N4" s="184"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -23519,21 +23519,21 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8">
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
+      <c r="F5" s="178"/>
+      <c r="G5" s="178"/>
+      <c r="H5" s="178"/>
+      <c r="I5" s="178"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="178"/>
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -23565,21 +23565,21 @@
       </c>
     </row>
     <row r="7" spans="2:27">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="178"/>
-      <c r="L7" s="178"/>
-      <c r="M7" s="178"/>
-      <c r="N7" s="178"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
+      <c r="L7" s="191"/>
+      <c r="M7" s="191"/>
+      <c r="N7" s="191"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -23605,11 +23605,11 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="2:27" ht="16.8">
-      <c r="B9" s="183" t="s">
+      <c r="B9" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="184"/>
-      <c r="D9" s="184"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
       <c r="E9" s="187" t="s">
         <v>14</v>
       </c>
@@ -23651,11 +23651,11 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="2:27" ht="16.8">
-      <c r="B11" s="183" t="s">
+      <c r="B11" s="177" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="184"/>
-      <c r="D11" s="184"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="187"/>
       <c r="F11" s="187"/>
       <c r="G11" s="187"/>
@@ -23672,42 +23672,42 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="2:27" ht="13.8">
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="184"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="184"/>
-      <c r="M12" s="184"/>
-      <c r="N12" s="184"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="178"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="178"/>
+      <c r="L12" s="178"/>
+      <c r="M12" s="178"/>
+      <c r="N12" s="178"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="2:27" ht="14.4" thickBot="1">
-      <c r="B13" s="190" t="s">
+      <c r="B13" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="191"/>
-      <c r="D13" s="191"/>
-      <c r="E13" s="191"/>
-      <c r="F13" s="191"/>
-      <c r="G13" s="191"/>
-      <c r="H13" s="191"/>
-      <c r="I13" s="191"/>
-      <c r="J13" s="191"/>
-      <c r="K13" s="191"/>
-      <c r="L13" s="191"/>
-      <c r="M13" s="191"/>
-      <c r="N13" s="191"/>
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="180"/>
+      <c r="M13" s="180"/>
+      <c r="N13" s="180"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -23717,10 +23717,10 @@
       <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="192" t="s">
+      <c r="C14" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="193"/>
+      <c r="D14" s="182"/>
       <c r="E14" s="45" t="s">
         <v>97</v>
       </c>
@@ -23758,8 +23758,8 @@
     </row>
     <row r="15" spans="2:27" hidden="1" thickBot="1">
       <c r="B15" s="11"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="195"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="184"/>
       <c r="E15" s="46"/>
       <c r="F15" s="46"/>
       <c r="G15" s="46"/>
@@ -27123,11 +27123,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:N12"/>
-    <mergeCell ref="B13:N13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B6:N6"/>
     <mergeCell ref="B8:N8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
@@ -27135,12 +27136,11 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="H11:N11"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="B6:N6"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:N12"/>
+    <mergeCell ref="B13:N13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <conditionalFormatting sqref="N16:N81">
     <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
@@ -27210,19 +27210,19 @@
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="2:27" ht="13.8">
-      <c r="B2" s="179"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="180"/>
-      <c r="I2" s="180"/>
-      <c r="J2" s="180"/>
-      <c r="K2" s="180"/>
-      <c r="L2" s="180"/>
-      <c r="M2" s="180"/>
-      <c r="N2" s="180"/>
+      <c r="B2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
+      <c r="M2" s="193"/>
+      <c r="N2" s="193"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -27232,21 +27232,21 @@
       </c>
     </row>
     <row r="3" spans="2:27" ht="18.600000000000001">
-      <c r="B3" s="181" t="s">
+      <c r="B3" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="182"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="182"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="182"/>
-      <c r="N3" s="182"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="195"/>
+      <c r="N3" s="195"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -27256,21 +27256,21 @@
       </c>
     </row>
     <row r="4" spans="2:27" ht="13.8">
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
-      <c r="K4" s="184"/>
-      <c r="L4" s="184"/>
-      <c r="M4" s="184"/>
-      <c r="N4" s="184"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="178"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
@@ -27280,21 +27280,21 @@
       </c>
     </row>
     <row r="5" spans="2:27" ht="13.8">
-      <c r="B5" s="183" t="s">
+      <c r="B5" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
+      <c r="F5" s="178"/>
+      <c r="G5" s="178"/>
+      <c r="H5" s="178"/>
+      <c r="I5" s="178"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="178"/>
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -27326,21 +27326,21 @@
       </c>
     </row>
     <row r="7" spans="2:27">
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="178"/>
-      <c r="K7" s="178"/>
-      <c r="L7" s="178"/>
-      <c r="M7" s="178"/>
-      <c r="N7" s="178"/>
+      <c r="C7" s="191"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="191"/>
+      <c r="L7" s="191"/>
+      <c r="M7" s="191"/>
+      <c r="N7" s="191"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -27366,11 +27366,11 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="2:27" ht="16.8">
-      <c r="B9" s="183" t="s">
+      <c r="B9" s="177" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="184"/>
-      <c r="D9" s="184"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
       <c r="E9" s="187" t="s">
         <v>14</v>
       </c>
@@ -27412,11 +27412,11 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="2:27" ht="16.8">
-      <c r="B11" s="183" t="s">
+      <c r="B11" s="177" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="184"/>
-      <c r="D11" s="184"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
       <c r="E11" s="187"/>
       <c r="F11" s="187"/>
       <c r="G11" s="187"/>
@@ -27433,42 +27433,42 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="2:27" ht="13.8">
-      <c r="B12" s="183" t="s">
+      <c r="B12" s="177" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="184"/>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="184"/>
-      <c r="M12" s="184"/>
-      <c r="N12" s="184"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="178"/>
+      <c r="J12" s="178"/>
+      <c r="K12" s="178"/>
+      <c r="L12" s="178"/>
+      <c r="M12" s="178"/>
+      <c r="N12" s="178"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="2:27" ht="14.4" thickBot="1">
-      <c r="B13" s="190" t="s">
+      <c r="B13" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="191"/>
-      <c r="D13" s="191"/>
-      <c r="E13" s="191"/>
-      <c r="F13" s="191"/>
-      <c r="G13" s="191"/>
-      <c r="H13" s="191"/>
-      <c r="I13" s="191"/>
-      <c r="J13" s="191"/>
-      <c r="K13" s="191"/>
-      <c r="L13" s="191"/>
-      <c r="M13" s="191"/>
-      <c r="N13" s="191"/>
+      <c r="C13" s="180"/>
+      <c r="D13" s="180"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="180"/>
+      <c r="M13" s="180"/>
+      <c r="N13" s="180"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -27478,10 +27478,10 @@
       <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="192" t="s">
+      <c r="C14" s="181" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="193"/>
+      <c r="D14" s="182"/>
       <c r="E14" s="45" t="s">
         <v>97</v>
       </c>
@@ -27519,8 +27519,8 @@
     </row>
     <row r="15" spans="2:27" hidden="1" thickBot="1">
       <c r="B15" s="11"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="195"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="184"/>
       <c r="E15" s="46"/>
       <c r="F15" s="46"/>
       <c r="G15" s="46"/>
@@ -30884,6 +30884,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E11:G11"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="E12:N12"/>
@@ -30900,8 +30902,6 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E11:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="N78:N81">
     <cfRule type="cellIs" dxfId="22" priority="5" operator="greaterThan">
@@ -72235,6 +72235,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D2009674D1E4E440A94D0AD297477650" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="53e0434df910c584ed32f9973a40d19f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="caf11648-aa17-4777-a2af-7bbeecc20fe5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5327aafdd5c8845bff671cc1d0921796" ns2:_="">
     <xsd:import namespace="caf11648-aa17-4777-a2af-7bbeecc20fe5"/>
@@ -72392,22 +72407,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{969EACA1-B7BE-4DA9-89BC-15B34C54129D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD9F7E5-D36C-48E0-ACE8-CFA8E8412A47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7051AAF9-05A6-40B0-B93C-E0A75ABB00E8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -72423,21 +72440,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD9F7E5-D36C-48E0-ACE8-CFA8E8412A47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{969EACA1-B7BE-4DA9-89BC-15B34C54129D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>